<commit_message>
tomk79\pickles2\pathResolver\main::resolve_common_contents() で、content が 0バイトのファイルの場合に異常終了する不具合を修正
</commit_message>
<xml_diff>
--- a/tests/testdata/standard/px-files/sitemaps/sitemap.xlsx
+++ b/tests/testdata/standard/px-files/sitemaps/sitemap.xlsx
@@ -15,15 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
-  <si>
-    <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+  <si>
+    <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.3</t>
   </si>
   <si>
     <t>「Pickles 2」 サイトマップ</t>
   </si>
   <si>
-    <t>Exported: 2016-01-02 06:33:34</t>
+    <t>Exported: 2016-07-23 02:09:43</t>
   </si>
   <si>
     <t>ページID</t>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>/index.html</t>
+  </si>
+  <si>
+    <t>Path TEST 0 bite</t>
+  </si>
+  <si>
+    <t>/path_test_0bite/</t>
+  </si>
+  <si>
+    <t>/0bite.html</t>
+  </si>
+  <si>
+    <t>Path TEST not exists</t>
+  </si>
+  <si>
+    <t>/path_test_not_exists/</t>
+  </si>
+  <si>
+    <t>/not_exists.html</t>
   </si>
   <si>
     <t>EndOfData</t>
@@ -619,7 +637,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
@@ -847,28 +865,94 @@
       </c>
       <c r="S10" s="4"/>
     </row>
-    <row r="13" spans="1:19" customHeight="1" ht="5">
-      <c r="A13" s="10" t="s">
+    <row r="11" spans="1:19">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="4">
+        <v>1</v>
+      </c>
+      <c r="S12" s="4"/>
+    </row>
+    <row r="15" spans="1:19" customHeight="1" ht="5">
+      <c r="A15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>